<commit_message>
12 years to a million, not 13
</commit_message>
<xml_diff>
--- a/assets/files/posts/2022/EasyRich.xlsx
+++ b/assets/files/posts/2022/EasyRich.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanm\git\easyrich\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanm\git\easyrich\assets\files\posts\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48953588-6215-4F0B-AE18-E72004E44298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06456CF-DE48-407C-BDC5-A3E1E60ECBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{24B1CF4B-5FFC-4CE4-B832-6C89CEF4C3CE}"/>
   </bookViews>
@@ -141,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,6 +154,8 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20" customBuiltin="1"/>
@@ -477,19 +479,18 @@
   <dimension ref="B2:R12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="15" width="8.796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -506,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4">
-        <v>48000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.45">
@@ -568,63 +569,63 @@
       </c>
       <c r="D7" s="5">
         <f>C10</f>
-        <v>48000</v>
+        <v>50000</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" ref="E7:R7" si="0">D10</f>
-        <v>99360</v>
+        <v>103500</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>154315.20000000001</v>
+        <v>160745</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>213117.26400000002</v>
+        <v>221997.15</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>276035.47248</v>
+        <v>287536.95050000004</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
-        <v>343357.95555359998</v>
+        <v>357664.53703500004</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
-        <v>415393.01244235196</v>
+        <v>432701.05462745007</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="0"/>
-        <v>492470.52331331657</v>
+        <v>512990.12845137157</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="0"/>
-        <v>574943.45994524879</v>
+        <v>598899.43744296755</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="0"/>
-        <v>663189.50214141619</v>
+        <v>690822.39806397527</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
-        <v>757612.76729131537</v>
+        <v>789179.96592845349</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>858645.66100170743</v>
+        <v>894422.5635434452</v>
       </c>
       <c r="P7" s="5">
         <f t="shared" si="0"/>
-        <v>966750.85727182694</v>
+        <v>1007032.1429914864</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="0"/>
-        <v>1082423.4172808549</v>
+        <v>1127524.3930008905</v>
       </c>
       <c r="R7" s="5">
         <f t="shared" si="0"/>
-        <v>1206193.0564905147</v>
+        <v>1256451.1005109528</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.45">
@@ -632,68 +633,68 @@
         <v>1</v>
       </c>
       <c r="C8" s="5">
-        <f>C7 * return</f>
+        <f t="shared" ref="C8:R8" si="1">C7 * return</f>
         <v>0</v>
       </c>
       <c r="D8" s="5">
-        <f>D7 * return</f>
-        <v>3360.0000000000005</v>
+        <f t="shared" si="1"/>
+        <v>3500.0000000000005</v>
       </c>
       <c r="E8" s="5">
-        <f>E7 * return</f>
-        <v>6955.2000000000007</v>
+        <f t="shared" si="1"/>
+        <v>7245.0000000000009</v>
       </c>
       <c r="F8" s="5">
-        <f>F7 * return</f>
-        <v>10802.064000000002</v>
+        <f t="shared" si="1"/>
+        <v>11252.150000000001</v>
       </c>
       <c r="G8" s="5">
-        <f>G7 * return</f>
-        <v>14918.208480000003</v>
+        <f t="shared" si="1"/>
+        <v>15539.800500000001</v>
       </c>
       <c r="H8" s="5">
-        <f>H7 * return</f>
-        <v>19322.4830736</v>
+        <f t="shared" si="1"/>
+        <v>20127.586535000006</v>
       </c>
       <c r="I8" s="5">
-        <f>I7 * return</f>
-        <v>24035.056888752002</v>
+        <f t="shared" si="1"/>
+        <v>25036.517592450007</v>
       </c>
       <c r="J8" s="5">
-        <f>J7 * return</f>
-        <v>29077.510870964641</v>
+        <f t="shared" si="1"/>
+        <v>30289.073823921506</v>
       </c>
       <c r="K8" s="5">
-        <f>K7 * return</f>
-        <v>34472.936631932163</v>
+        <f t="shared" si="1"/>
+        <v>35909.308991596015</v>
       </c>
       <c r="L8" s="5">
-        <f>L7 * return</f>
-        <v>40246.042196167422</v>
+        <f t="shared" si="1"/>
+        <v>41922.960621007733</v>
       </c>
       <c r="M8" s="5">
-        <f>M7 * return</f>
-        <v>46423.26514989914</v>
+        <f t="shared" si="1"/>
+        <v>48357.567864478275</v>
       </c>
       <c r="N8" s="5">
-        <f>N7 * return</f>
-        <v>53032.893710392083</v>
+        <f t="shared" si="1"/>
+        <v>55242.597614991748</v>
       </c>
       <c r="O8" s="5">
-        <f>O7 * return</f>
-        <v>60105.196270119523</v>
+        <f t="shared" si="1"/>
+        <v>62609.579448041171</v>
       </c>
       <c r="P8" s="5">
-        <f>P7 * return</f>
-        <v>67672.560009027889</v>
+        <f t="shared" si="1"/>
+        <v>70492.250009404059</v>
       </c>
       <c r="Q8" s="5">
-        <f>Q7 * return</f>
-        <v>75769.639209659843</v>
+        <f t="shared" si="1"/>
+        <v>78926.707510062348</v>
       </c>
       <c r="R8" s="5">
-        <f>R7 * return</f>
-        <v>84433.513954336027</v>
+        <f t="shared" si="1"/>
+        <v>87951.577035766706</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.45">
@@ -701,68 +702,68 @@
         <v>3</v>
       </c>
       <c r="C9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" ref="C9:R9" si="2">savings</f>
+        <v>50000</v>
       </c>
       <c r="D9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="E9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="F9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="G9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="H9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="I9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="J9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="K9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="L9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="M9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="N9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="O9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="P9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="Q9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
       <c r="R9" s="5">
-        <f>savings</f>
-        <v>48000</v>
+        <f t="shared" si="2"/>
+        <v>50000</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.45">
@@ -771,67 +772,67 @@
       </c>
       <c r="C10" s="6">
         <f>C7 + C8 + C9</f>
-        <v>48000</v>
+        <v>50000</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" ref="D10" si="1">D7 + D8 + D9</f>
-        <v>99360</v>
+        <f t="shared" ref="D10" si="3">D7 + D8 + D9</f>
+        <v>103500</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" ref="E10" si="2">E7 + E8 + E9</f>
-        <v>154315.20000000001</v>
+        <f t="shared" ref="E10" si="4">E7 + E8 + E9</f>
+        <v>160745</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" ref="F10" si="3">F7 + F8 + F9</f>
-        <v>213117.26400000002</v>
+        <f t="shared" ref="F10" si="5">F7 + F8 + F9</f>
+        <v>221997.15</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" ref="G10" si="4">G7 + G8 + G9</f>
-        <v>276035.47248</v>
+        <f t="shared" ref="G10" si="6">G7 + G8 + G9</f>
+        <v>287536.95050000004</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10" si="5">H7 + H8 + H9</f>
-        <v>343357.95555359998</v>
+        <f t="shared" ref="H10" si="7">H7 + H8 + H9</f>
+        <v>357664.53703500004</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" ref="I10" si="6">I7 + I8 + I9</f>
-        <v>415393.01244235196</v>
+        <f t="shared" ref="I10" si="8">I7 + I8 + I9</f>
+        <v>432701.05462745007</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" ref="J10" si="7">J7 + J8 + J9</f>
-        <v>492470.52331331657</v>
+        <f t="shared" ref="J10" si="9">J7 + J8 + J9</f>
+        <v>512990.12845137157</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" ref="K10" si="8">K7 + K8 + K9</f>
-        <v>574943.45994524879</v>
+        <f t="shared" ref="K10" si="10">K7 + K8 + K9</f>
+        <v>598899.43744296755</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" ref="L10" si="9">L7 + L8 + L9</f>
-        <v>663189.50214141619</v>
+        <f t="shared" ref="L10" si="11">L7 + L8 + L9</f>
+        <v>690822.39806397527</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" ref="M10" si="10">M7 + M8 + M9</f>
-        <v>757612.76729131537</v>
+        <f t="shared" ref="M10" si="12">M7 + M8 + M9</f>
+        <v>789179.96592845349</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" ref="N10" si="11">N7 + N8 + N9</f>
-        <v>858645.66100170743</v>
-      </c>
-      <c r="O10" s="6">
-        <f t="shared" ref="O10" si="12">O7 + O8 + O9</f>
-        <v>966750.85727182694</v>
-      </c>
-      <c r="P10" s="7">
-        <f t="shared" ref="P10" si="13">P7 + P8 + P9</f>
-        <v>1082423.4172808549</v>
+        <f t="shared" ref="N10" si="13">N7 + N8 + N9</f>
+        <v>894422.5635434452</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" ref="O10" si="14">O7 + O8 + O9</f>
+        <v>1007032.1429914864</v>
+      </c>
+      <c r="P10" s="8">
+        <f t="shared" ref="P10" si="15">P7 + P8 + P9</f>
+        <v>1127524.3930008905</v>
       </c>
       <c r="Q10" s="6">
-        <f t="shared" ref="Q10" si="14">Q7 + Q8 + Q9</f>
-        <v>1206193.0564905147</v>
+        <f t="shared" ref="Q10" si="16">Q7 + Q8 + Q9</f>
+        <v>1256451.1005109528</v>
       </c>
       <c r="R10" s="6">
-        <f t="shared" ref="R10" si="15">R7 + R8 + R9</f>
-        <v>1338626.5704448507</v>
+        <f t="shared" ref="R10" si="17">R7 + R8 + R9</f>
+        <v>1394402.6775467196</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
extended model to 30 years
</commit_message>
<xml_diff>
--- a/assets/files/posts/2022/EasyRich.xlsx
+++ b/assets/files/posts/2022/EasyRich.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanm\git\easyrich\assets\files\posts\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06456CF-DE48-407C-BDC5-A3E1E60ECBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7707FF-FB53-40DF-9D93-C7EAEC1082F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{24B1CF4B-5FFC-4CE4-B832-6C89CEF4C3CE}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{24B1CF4B-5FFC-4CE4-B832-6C89CEF4C3CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" r:id="rId1"/>
@@ -476,25 +476,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C794AC63-3D4D-4E32-B458-37C71CAC4D24}">
-  <dimension ref="B2:R12"/>
+  <dimension ref="B2:AG12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="10.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="14" width="8.796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="33" width="10.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.45">
       <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -502,7 +502,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -510,7 +510,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.45">
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -559,8 +559,53 @@
       <c r="R6" s="1">
         <v>15</v>
       </c>
+      <c r="S6" s="1">
+        <v>16</v>
+      </c>
+      <c r="T6" s="1">
+        <v>17</v>
+      </c>
+      <c r="U6" s="1">
+        <v>18</v>
+      </c>
+      <c r="V6" s="1">
+        <v>19</v>
+      </c>
+      <c r="W6" s="1">
+        <v>20</v>
+      </c>
+      <c r="X6" s="1">
+        <v>21</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>22</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>23</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>25</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>26</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>27</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>28</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>29</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,146 +672,326 @@
         <f t="shared" si="0"/>
         <v>1256451.1005109528</v>
       </c>
+      <c r="S7" s="5">
+        <f t="shared" ref="S7" si="1">R10</f>
+        <v>1394402.6775467196</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" ref="T7" si="2">S10</f>
+        <v>1542010.86497499</v>
+      </c>
+      <c r="U7" s="5">
+        <f t="shared" ref="U7" si="3">T10</f>
+        <v>1699951.6255232394</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" ref="V7" si="4">U10</f>
+        <v>1868948.2393098662</v>
+      </c>
+      <c r="W7" s="5">
+        <f t="shared" ref="W7" si="5">V10</f>
+        <v>2049774.6160615569</v>
+      </c>
+      <c r="X7" s="5">
+        <f t="shared" ref="X7" si="6">W10</f>
+        <v>2243258.8391858661</v>
+      </c>
+      <c r="Y7" s="5">
+        <f t="shared" ref="Y7" si="7">X10</f>
+        <v>2450286.9579288769</v>
+      </c>
+      <c r="Z7" s="5">
+        <f t="shared" ref="Z7" si="8">Y10</f>
+        <v>2671807.0449838983</v>
+      </c>
+      <c r="AA7" s="5">
+        <f t="shared" ref="AA7" si="9">Z10</f>
+        <v>2908833.5381327714</v>
+      </c>
+      <c r="AB7" s="5">
+        <f t="shared" ref="AB7" si="10">AA10</f>
+        <v>3162451.8858020655</v>
+      </c>
+      <c r="AC7" s="5">
+        <f t="shared" ref="AC7" si="11">AB10</f>
+        <v>3433823.5178082101</v>
+      </c>
+      <c r="AD7" s="5">
+        <f t="shared" ref="AD7" si="12">AC10</f>
+        <v>3724191.1640547849</v>
+      </c>
+      <c r="AE7" s="5">
+        <f t="shared" ref="AE7" si="13">AD10</f>
+        <v>4034884.5455386201</v>
+      </c>
+      <c r="AF7" s="5">
+        <f t="shared" ref="AF7" si="14">AE10</f>
+        <v>4367326.4637263231</v>
+      </c>
+      <c r="AG7" s="5">
+        <f t="shared" ref="AG7" si="15">AF10</f>
+        <v>4723039.3161871657</v>
+      </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" ref="C8:R8" si="1">C7 * return</f>
+        <f t="shared" ref="C8:R8" si="16">C7 * return</f>
         <v>0</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>3500.0000000000005</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>7245.0000000000009</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>11252.150000000001</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>15539.800500000001</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>20127.586535000006</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>25036.517592450007</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>30289.073823921506</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>35909.308991596015</v>
       </c>
       <c r="L8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>41922.960621007733</v>
       </c>
       <c r="M8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>48357.567864478275</v>
       </c>
       <c r="N8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>55242.597614991748</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>62609.579448041171</v>
       </c>
       <c r="P8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>70492.250009404059</v>
       </c>
       <c r="Q8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>78926.707510062348</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>87951.577035766706</v>
       </c>
+      <c r="S8" s="5">
+        <f t="shared" ref="S8:AG8" si="17">S7 * return</f>
+        <v>97608.187428270379</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="17"/>
+        <v>107940.76054824931</v>
+      </c>
+      <c r="U8" s="5">
+        <f t="shared" si="17"/>
+        <v>118996.61378662677</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="17"/>
+        <v>130826.37675169065</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="17"/>
+        <v>143484.22312430901</v>
+      </c>
+      <c r="X8" s="5">
+        <f t="shared" si="17"/>
+        <v>157028.11874301065</v>
+      </c>
+      <c r="Y8" s="5">
+        <f t="shared" si="17"/>
+        <v>171520.0870550214</v>
+      </c>
+      <c r="Z8" s="5">
+        <f t="shared" si="17"/>
+        <v>187026.49314887289</v>
+      </c>
+      <c r="AA8" s="5">
+        <f t="shared" si="17"/>
+        <v>203618.34766929402</v>
+      </c>
+      <c r="AB8" s="5">
+        <f t="shared" si="17"/>
+        <v>221371.63200614462</v>
+      </c>
+      <c r="AC8" s="5">
+        <f t="shared" si="17"/>
+        <v>240367.64624657473</v>
+      </c>
+      <c r="AD8" s="5">
+        <f t="shared" si="17"/>
+        <v>260693.38148383496</v>
+      </c>
+      <c r="AE8" s="5">
+        <f t="shared" si="17"/>
+        <v>282441.91818770341</v>
+      </c>
+      <c r="AF8" s="5">
+        <f t="shared" si="17"/>
+        <v>305712.85246084264</v>
+      </c>
+      <c r="AG8" s="5">
+        <f t="shared" si="17"/>
+        <v>330612.75213310163</v>
+      </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" ref="C9:R9" si="2">savings</f>
+        <f t="shared" ref="C9:AG9" si="18">savings</f>
         <v>50000</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="L9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="N9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="P9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="Q9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="S9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="U9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="V9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="W9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="X9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="Y9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="Z9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AA9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AB9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AC9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AD9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AE9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AF9" s="5">
+        <f t="shared" si="18"/>
+        <v>50000</v>
+      </c>
+      <c r="AG9" s="5">
+        <f t="shared" si="18"/>
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
@@ -775,72 +1000,132 @@
         <v>50000</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" ref="D10" si="3">D7 + D8 + D9</f>
+        <f t="shared" ref="D10" si="19">D7 + D8 + D9</f>
         <v>103500</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" ref="E10" si="4">E7 + E8 + E9</f>
+        <f t="shared" ref="E10" si="20">E7 + E8 + E9</f>
         <v>160745</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" ref="F10" si="5">F7 + F8 + F9</f>
+        <f t="shared" ref="F10" si="21">F7 + F8 + F9</f>
         <v>221997.15</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" ref="G10" si="6">G7 + G8 + G9</f>
+        <f t="shared" ref="G10" si="22">G7 + G8 + G9</f>
         <v>287536.95050000004</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10" si="7">H7 + H8 + H9</f>
+        <f t="shared" ref="H10" si="23">H7 + H8 + H9</f>
         <v>357664.53703500004</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" ref="I10" si="8">I7 + I8 + I9</f>
+        <f t="shared" ref="I10" si="24">I7 + I8 + I9</f>
         <v>432701.05462745007</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" ref="J10" si="9">J7 + J8 + J9</f>
+        <f t="shared" ref="J10" si="25">J7 + J8 + J9</f>
         <v>512990.12845137157</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" ref="K10" si="10">K7 + K8 + K9</f>
+        <f t="shared" ref="K10" si="26">K7 + K8 + K9</f>
         <v>598899.43744296755</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" ref="L10" si="11">L7 + L8 + L9</f>
+        <f t="shared" ref="L10" si="27">L7 + L8 + L9</f>
         <v>690822.39806397527</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" ref="M10" si="12">M7 + M8 + M9</f>
+        <f t="shared" ref="M10" si="28">M7 + M8 + M9</f>
         <v>789179.96592845349</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" ref="N10" si="13">N7 + N8 + N9</f>
+        <f t="shared" ref="N10" si="29">N7 + N8 + N9</f>
         <v>894422.5635434452</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" ref="O10" si="14">O7 + O8 + O9</f>
+        <f t="shared" ref="O10" si="30">O7 + O8 + O9</f>
         <v>1007032.1429914864</v>
       </c>
       <c r="P10" s="8">
-        <f t="shared" ref="P10" si="15">P7 + P8 + P9</f>
+        <f t="shared" ref="P10" si="31">P7 + P8 + P9</f>
         <v>1127524.3930008905</v>
       </c>
       <c r="Q10" s="6">
-        <f t="shared" ref="Q10" si="16">Q7 + Q8 + Q9</f>
+        <f t="shared" ref="Q10:AG10" si="32">Q7 + Q8 + Q9</f>
         <v>1256451.1005109528</v>
       </c>
       <c r="R10" s="6">
-        <f t="shared" ref="R10" si="17">R7 + R8 + R9</f>
+        <f t="shared" ref="R10:AF10" si="33">R7 + R8 + R9</f>
         <v>1394402.6775467196</v>
       </c>
+      <c r="S10" s="6">
+        <f t="shared" si="32"/>
+        <v>1542010.86497499</v>
+      </c>
+      <c r="T10" s="6">
+        <f t="shared" si="33"/>
+        <v>1699951.6255232394</v>
+      </c>
+      <c r="U10" s="6">
+        <f t="shared" si="32"/>
+        <v>1868948.2393098662</v>
+      </c>
+      <c r="V10" s="6">
+        <f t="shared" si="33"/>
+        <v>2049774.6160615569</v>
+      </c>
+      <c r="W10" s="6">
+        <f t="shared" si="32"/>
+        <v>2243258.8391858661</v>
+      </c>
+      <c r="X10" s="6">
+        <f t="shared" si="33"/>
+        <v>2450286.9579288769</v>
+      </c>
+      <c r="Y10" s="6">
+        <f t="shared" si="32"/>
+        <v>2671807.0449838983</v>
+      </c>
+      <c r="Z10" s="6">
+        <f t="shared" si="33"/>
+        <v>2908833.5381327714</v>
+      </c>
+      <c r="AA10" s="6">
+        <f t="shared" si="32"/>
+        <v>3162451.8858020655</v>
+      </c>
+      <c r="AB10" s="6">
+        <f t="shared" si="33"/>
+        <v>3433823.5178082101</v>
+      </c>
+      <c r="AC10" s="6">
+        <f t="shared" si="32"/>
+        <v>3724191.1640547849</v>
+      </c>
+      <c r="AD10" s="6">
+        <f t="shared" si="33"/>
+        <v>4034884.5455386201</v>
+      </c>
+      <c r="AE10" s="6">
+        <f t="shared" si="32"/>
+        <v>4367326.4637263231</v>
+      </c>
+      <c r="AF10" s="6">
+        <f t="shared" si="33"/>
+        <v>4723039.3161871657</v>
+      </c>
+      <c r="AG10" s="6">
+        <f t="shared" si="32"/>
+        <v>5103652.0683202669</v>
+      </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B12" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C10:R10">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C10:AG10">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -849,8 +1134,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:R8">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C8:AG8">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>